<commit_message>
Updated result for RQ1 of Freecol.
</commit_message>
<xml_diff>
--- a/Results of iClones.xlsx
+++ b/Results of iClones.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCD4310-8EB1-4387-8692-C21498E3B13E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE77C40-EE98-43D2-82B8-51AF72FC1A18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12930" yWindow="7035" windowWidth="14925" windowHeight="6015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12480" yWindow="5385" windowWidth="14925" windowHeight="6015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
@@ -808,7 +808,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,21 +879,21 @@
         <v>32</v>
       </c>
       <c r="D3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <f>C3/D3</f>
-        <v>2.4615384615384617</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3">
         <f>F3/G3</f>
-        <v>0.15384615384615385</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -931,13 +931,25 @@
       <c r="B5">
         <v>10354</v>
       </c>
-      <c r="E5" t="e">
+      <c r="C5">
+        <v>1751</v>
+      </c>
+      <c r="D5">
+        <v>93</v>
+      </c>
+      <c r="E5">
         <f>C5/D5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H5" t="e">
+        <v>18.827956989247312</v>
+      </c>
+      <c r="F5">
+        <v>67</v>
+      </c>
+      <c r="G5">
+        <v>93</v>
+      </c>
+      <c r="H5">
         <f>F5/G5</f>
-        <v>#DIV/0!</v>
+        <v>0.72043010752688175</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -967,21 +979,21 @@
         <v>171</v>
       </c>
       <c r="D7">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7">
         <f>C7/D7</f>
-        <v>4.75</v>
+        <v>4.8857142857142861</v>
       </c>
       <c r="F7">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G7">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H7">
         <f>F7/G7</f>
-        <v>0.3888888888888889</v>
+        <v>0.22857142857142856</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -990,27 +1002,27 @@
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>236</v>
+        <v>1987</v>
       </c>
       <c r="D8">
         <f>SUM(D3:D7)</f>
-        <v>59</v>
+        <v>150</v>
       </c>
       <c r="E8">
         <f>C8/D8</f>
-        <v>4</v>
+        <v>13.246666666666666</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="G8">
         <f>SUM(G3:G7)</f>
-        <v>59</v>
+        <v>150</v>
       </c>
       <c r="H8">
         <f>F8/G8</f>
-        <v>0.2711864406779661</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1058,7 +1070,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,9 +1118,21 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="e">
+      <c r="B3">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <v>32</v>
+      </c>
+      <c r="D3">
         <f>B3/C3*100</f>
-        <v>#DIV/0!</v>
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
       </c>
       <c r="G3" t="e">
         <f>E3/F3*100</f>
@@ -1119,9 +1143,21 @@
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="e">
+      <c r="B4">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>36</v>
+      </c>
+      <c r="D4">
         <f t="shared" ref="D4" si="0">B4/C4*100</f>
-        <v>#DIV/0!</v>
+        <v>91.666666666666657</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
       </c>
       <c r="G4" t="e">
         <f t="shared" ref="G4" si="1">E4/F4*100</f>
@@ -1158,13 +1194,25 @@
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="e">
+      <c r="B7">
+        <v>171</v>
+      </c>
+      <c r="C7">
+        <v>198</v>
+      </c>
+      <c r="D7">
         <f>B7/C7*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G7" t="e">
+        <v>86.36363636363636</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+      <c r="G7">
         <f>E7/F7*100</f>
-        <v>#DIV/0!</v>
+        <v>88.888888888888886</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1173,27 +1221,27 @@
       </c>
       <c r="B8">
         <f>SUM(B3:B7)</f>
-        <v>0</v>
+        <v>236</v>
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" t="e">
+        <v>266</v>
+      </c>
+      <c r="D8">
         <f>B8/C8*100</f>
-        <v>#DIV/0!</v>
+        <v>88.721804511278194</v>
       </c>
       <c r="E8">
         <f>SUM(E3:E7)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" t="e">
+        <v>9</v>
+      </c>
+      <c r="G8">
         <f>E8/F8*100</f>
-        <v>#DIV/0!</v>
+        <v>88.888888888888886</v>
       </c>
     </row>
   </sheetData>
@@ -1211,7 +1259,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,26 +1308,50 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="e">
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
         <f>B3/C3*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G3" t="e">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <f>E3/F3*100</f>
-        <v>#DIV/0!</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="e">
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
         <f t="shared" ref="D4" si="0">B4/C4*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" t="e">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <f t="shared" ref="G4" si="1">E4/F4*100</f>
-        <v>#DIV/0!</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1312,13 +1384,25 @@
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="e">
+      <c r="B7">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>36</v>
+      </c>
+      <c r="D7">
         <f>B7/C7*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G7" t="e">
+        <v>97.222222222222214</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
         <f>E7/F7*100</f>
-        <v>#DIV/0!</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1327,27 +1411,27 @@
       </c>
       <c r="B8">
         <f>SUM(B3:B7)</f>
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" t="e">
+        <v>58</v>
+      </c>
+      <c r="D8">
         <f>B8/C8*100</f>
-        <v>#DIV/0!</v>
+        <v>98.275862068965509</v>
       </c>
       <c r="E8">
         <f>SUM(E3:E7)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" t="e">
+        <v>5</v>
+      </c>
+      <c r="G8">
         <f>E8/F8*100</f>
-        <v>#DIV/0!</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1365,7 +1449,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,26 +1499,50 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="e">
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
         <f>C3/B3*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G3" t="e">
+        <v>41.666666666666671</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <f>F3/E3*100</f>
-        <v>#DIV/0!</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="e">
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
         <f t="shared" ref="D4" si="0">C4/B4*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" t="e">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <f t="shared" ref="G4" si="1">F4/E4*100</f>
-        <v>#DIV/0!</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1482,27 +1590,27 @@
       </c>
       <c r="B8">
         <f>SUM(B3:B7)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" t="e">
+        <v>7</v>
+      </c>
+      <c r="D8">
         <f>C8/B8*100</f>
-        <v>#DIV/0!</v>
+        <v>31.818181818181817</v>
       </c>
       <c r="E8">
         <f>SUM(E3:E7)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" t="e">
+        <v>2</v>
+      </c>
+      <c r="G8">
         <f>F8/E8*100</f>
-        <v>#DIV/0!</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Solved the problem with null pointer exception.
</commit_message>
<xml_diff>
--- a/Results of iClones.xlsx
+++ b/Results of iClones.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE77C40-EE98-43D2-82B8-51AF72FC1A18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489A39E5-CB8D-4541-80B4-555EF2EAF238}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12480" yWindow="5385" windowWidth="14925" windowHeight="6015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12630" yWindow="480" windowWidth="14925" windowHeight="6015" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,13 +959,25 @@
       <c r="B6">
         <v>2886</v>
       </c>
-      <c r="E6" t="e">
+      <c r="C6">
+        <v>298</v>
+      </c>
+      <c r="D6">
+        <v>24</v>
+      </c>
+      <c r="E6">
         <f>C6/D6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H6" t="e">
+        <v>12.416666666666666</v>
+      </c>
+      <c r="F6">
+        <v>22</v>
+      </c>
+      <c r="G6">
+        <v>24</v>
+      </c>
+      <c r="H6">
         <f>F6/G6</f>
-        <v>#DIV/0!</v>
+        <v>0.91666666666666663</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -986,14 +998,14 @@
         <v>4.8857142857142861</v>
       </c>
       <c r="F7">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G7">
         <v>35</v>
       </c>
       <c r="H7">
         <f>F7/G7</f>
-        <v>0.22857142857142856</v>
+        <v>0.2857142857142857</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1002,27 +1014,27 @@
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>1987</v>
+        <v>2285</v>
       </c>
       <c r="D8">
         <f>SUM(D3:D7)</f>
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="E8">
         <f>C8/D8</f>
-        <v>13.246666666666666</v>
+        <v>13.132183908045977</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="G8">
         <f>SUM(G3:G7)</f>
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="H8">
         <f>F8/G8</f>
-        <v>0.5</v>
+        <v>0.56896551724137934</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1259,7 +1271,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45DAA6C-6044-4BDB-98CB-11DB5B63E69A}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,13 +1587,25 @@
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="e">
+      <c r="B7">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
         <f>C7/B7*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G7" t="e">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
         <f>F7/E7*100</f>
-        <v>#DIV/0!</v>
+        <v>66.666666666666657</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1590,27 +1614,27 @@
       </c>
       <c r="B8">
         <f>SUM(B3:B7)</f>
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <f>C8/B8*100</f>
-        <v>31.818181818181817</v>
+        <v>24.561403508771928</v>
       </c>
       <c r="E8">
         <f>SUM(E3:E7)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G8">
         <f>F8/E8*100</f>
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated for reduced number of revision.
</commit_message>
<xml_diff>
--- a/Results of iClones.xlsx
+++ b/Results of iClones.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09680013-6F6A-45B4-8070-C07582B53414}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC7C114-0F61-41CF-AA52-6E3A17ABA45A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12405" yWindow="1545" windowWidth="14925" windowHeight="6015" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11115" yWindow="2100" windowWidth="14925" windowHeight="7785" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
@@ -421,7 +421,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +694,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,12 +1336,13 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1383,65 +1384,125 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="e">
+      <c r="B3">
+        <v>62554</v>
+      </c>
+      <c r="C3">
+        <v>1944358</v>
+      </c>
+      <c r="D3">
         <f>B3/C3*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G3" t="e">
+        <v>3.2172058849244838</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>293188</v>
+      </c>
+      <c r="G3">
         <f>E3/F3*100</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="e">
+      <c r="B4">
+        <v>244275</v>
+      </c>
+      <c r="C4">
+        <v>6140060</v>
+      </c>
+      <c r="D4">
         <f t="shared" ref="D4" si="0">B4/C4*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" t="e">
+        <v>3.978381318749328</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>611781</v>
+      </c>
+      <c r="G4">
         <f t="shared" ref="G4" si="1">E4/F4*100</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" t="e">
+      <c r="B5">
+        <v>29761655</v>
+      </c>
+      <c r="C5">
+        <v>184093488</v>
+      </c>
+      <c r="D5">
         <f>B5/C5*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G5" t="e">
+        <v>16.166598462190038</v>
+      </c>
+      <c r="E5">
+        <v>167169</v>
+      </c>
+      <c r="F5">
+        <v>23887283</v>
+      </c>
+      <c r="G5">
         <f>E5/F5*100</f>
-        <v>#DIV/0!</v>
+        <v>0.6998242537671614</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="e">
+      <c r="B6">
+        <v>1556265</v>
+      </c>
+      <c r="C6">
+        <v>13666994</v>
+      </c>
+      <c r="D6">
         <f>B6/C6*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G6" t="e">
+        <v>11.387032144742289</v>
+      </c>
+      <c r="E6">
+        <v>5868</v>
+      </c>
+      <c r="F6">
+        <v>910632</v>
+      </c>
+      <c r="G6">
         <f>E6/F6*100</f>
-        <v>#DIV/0!</v>
+        <v>0.64438763408270305</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="e">
+      <c r="B7">
+        <v>2973484</v>
+      </c>
+      <c r="C7">
+        <v>40304299</v>
+      </c>
+      <c r="D7">
         <f>B7/C7*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G7" t="e">
+        <v>7.3775852049926485</v>
+      </c>
+      <c r="E7">
+        <v>5856</v>
+      </c>
+      <c r="F7">
+        <v>2304168</v>
+      </c>
+      <c r="G7">
         <f>E7/F7*100</f>
-        <v>#DIV/0!</v>
+        <v>0.2541481350318206</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1450,27 +1511,27 @@
       </c>
       <c r="B8">
         <f>SUM(B3:B7)</f>
-        <v>0</v>
+        <v>34598233</v>
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" t="e">
+        <v>246149199</v>
+      </c>
+      <c r="D8">
         <f>B8/C8*100</f>
-        <v>#DIV/0!</v>
+        <v>14.055797516529802</v>
       </c>
       <c r="E8">
         <f>SUM(E3:E7)</f>
-        <v>0</v>
+        <v>178893</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" t="e">
+        <v>28007052</v>
+      </c>
+      <c r="G8">
         <f>E8/F8*100</f>
-        <v>#DIV/0!</v>
+        <v>0.63874269951725016</v>
       </c>
     </row>
   </sheetData>

</xml_diff>